<commit_message>
Added a bit more
</commit_message>
<xml_diff>
--- a/Spreadsheet/Analytics.xlsx
+++ b/Spreadsheet/Analytics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GabrielJuarez/Documents/GitHub/MedievalPrime/Spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152D8EBC-137E-614C-9536-9EB68D51EB64}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4732ED15-6C73-D243-ADF2-53C6AE46C9B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
   <si>
     <t>Retention (# of players that keep coming back)</t>
   </si>
@@ -117,8 +117,56 @@
     <t>8th town</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"># of tries player took to get to </t>
+    <t>Armor 1</t>
+  </si>
+  <si>
+    <t>Armor 2</t>
+  </si>
+  <si>
+    <t>Armor 3</t>
+  </si>
+  <si>
+    <t>Armor 4</t>
+  </si>
+  <si>
+    <t>Weapon 1</t>
+  </si>
+  <si>
+    <t>Weapon 2</t>
+  </si>
+  <si>
+    <t>Weapon 3</t>
+  </si>
+  <si>
+    <t>Weapon 4</t>
+  </si>
+  <si>
+    <t>Character 1</t>
+  </si>
+  <si>
+    <t>Character 2</t>
+  </si>
+  <si>
+    <t>Character 3</t>
+  </si>
+  <si>
+    <t>Character 4</t>
+  </si>
+  <si>
+    <t># of players that bought these items</t>
+  </si>
+  <si>
+    <t># of players that redeemed these items using collectibles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># of players that won these items in chests </t>
+  </si>
+  <si>
+    <t># of players that sold these items?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># of tries player(s) took to get to </t>
     </r>
     <r>
       <rPr>
@@ -144,7 +192,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve"># of coins earned after </t>
+      <t xml:space="preserve"># of times player(s) chose to go back and cash-out after </t>
     </r>
     <r>
       <rPr>
@@ -170,7 +218,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve"># of times player chose to go back and cash-out after </t>
+      <t xml:space="preserve"># of messages the player(s) delivered after </t>
     </r>
     <r>
       <rPr>
@@ -196,7 +244,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve"># of messages delivered after </t>
+      <t xml:space="preserve"># of coins the player(s) earned after </t>
     </r>
     <r>
       <rPr>
@@ -222,7 +270,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve"># of coins spent at </t>
+      <t xml:space="preserve"># of coins the player(s) spent at </t>
     </r>
     <r>
       <rPr>
@@ -248,7 +296,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve"># of items &amp; collectibles obtained at </t>
+      <t xml:space="preserve"># of items &amp; collectibles the player(s) obtained at </t>
     </r>
     <r>
       <rPr>
@@ -274,7 +322,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve"># of boosts player used to get to </t>
+      <t xml:space="preserve"># of boosts the player(s) used to get to </t>
     </r>
     <r>
       <rPr>
@@ -297,6 +345,160 @@
       </rPr>
       <t xml:space="preserve"> town</t>
     </r>
+  </si>
+  <si>
+    <t>Boost 1</t>
+  </si>
+  <si>
+    <t>Boost 2</t>
+  </si>
+  <si>
+    <t>Boost 3</t>
+  </si>
+  <si>
+    <t>Boost 4</t>
+  </si>
+  <si>
+    <t>Collectible 1</t>
+  </si>
+  <si>
+    <t>Collectible 2</t>
+  </si>
+  <si>
+    <t>Collectible 3</t>
+  </si>
+  <si>
+    <t>Collectible 4</t>
+  </si>
+  <si>
+    <t>Collectible 5</t>
+  </si>
+  <si>
+    <t>Collectible 6</t>
+  </si>
+  <si>
+    <t>Collectible 7</t>
+  </si>
+  <si>
+    <t>Collectible 8</t>
+  </si>
+  <si>
+    <t>Collectible 9</t>
+  </si>
+  <si>
+    <t>Collectible 10</t>
+  </si>
+  <si>
+    <t>Collectible 11</t>
+  </si>
+  <si>
+    <t>Collectible 12</t>
+  </si>
+  <si>
+    <t>Player Runner Analytics</t>
+  </si>
+  <si>
+    <t># of players that bought these collectible</t>
+  </si>
+  <si>
+    <t># of players that used these collectible to redeem an item</t>
+  </si>
+  <si>
+    <t># of players that won these items in a chest</t>
+  </si>
+  <si>
+    <t>Collectibles Used Among Players</t>
+  </si>
+  <si>
+    <t>Items (i.e. armor, weapons, character skins, boosts) Used Among Players</t>
+  </si>
+  <si>
+    <t>Skill 1</t>
+  </si>
+  <si>
+    <t>Skill 2</t>
+  </si>
+  <si>
+    <t>Skill 3</t>
+  </si>
+  <si>
+    <t>Skill 4</t>
+  </si>
+  <si>
+    <t>Skill 5</t>
+  </si>
+  <si>
+    <t>Skill 6</t>
+  </si>
+  <si>
+    <t>Skill 7</t>
+  </si>
+  <si>
+    <t>Skill 8</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># of players that upgraded </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> skill</t>
+    </r>
+  </si>
+  <si>
+    <t># of players that traded these items??</t>
+  </si>
+  <si>
+    <t># of players that traded these collectibles ??</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Time (in min/sec) the player(s) spent on the run to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> town</t>
+    </r>
+  </si>
+  <si>
+    <t>Home-town/base Analytics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time (in min/sec) the player(s) spent at home-town </t>
   </si>
 </sst>
 </file>
@@ -348,7 +550,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -371,17 +573,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -392,6 +624,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,22 +930,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:R32"/>
+  <dimension ref="B5:AE38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -726,16 +984,16 @@
       <c r="F8" s="1"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
@@ -785,19 +1043,19 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
         <v>16</v>
@@ -818,7 +1076,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>5</v>
       </c>
@@ -829,7 +1087,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
@@ -840,42 +1098,113 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7" t="s">
+    <row r="24" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N24" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="O24" s="9"/>
+      <c r="P24" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q24" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="R24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="S24" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="T24" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="U24" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="V24" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="W24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="X24" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y24" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z24" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA24" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB24" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC24" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD24" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE24" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:31" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I25" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="J25" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-    </row>
-    <row r="26" spans="2:18" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="8"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="16"/>
+      <c r="AA25" s="16"/>
+      <c r="AB25" s="16"/>
+      <c r="AC25" s="16"/>
+      <c r="AD25" s="16"/>
+      <c r="AE25" s="16"/>
+    </row>
+    <row r="26" spans="2:31" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="7"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -884,12 +1213,32 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="2:18" ht="112" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="8"/>
+      <c r="N26" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O26" s="7"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+    </row>
+    <row r="27" spans="2:31" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="7"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -898,12 +1247,32 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="2:18" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="9"/>
+      <c r="N27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O27" s="7"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+    </row>
+    <row r="28" spans="2:31" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="8"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -912,12 +1281,32 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="2:18" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="8"/>
+      <c r="N28" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O28" s="7"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+    </row>
+    <row r="29" spans="2:31" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="7"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -926,12 +1315,32 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="2:18" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="8"/>
+      <c r="N29" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="O29" s="7"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+    </row>
+    <row r="30" spans="2:31" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="7"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -940,12 +1349,32 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="2:18" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="8"/>
+      <c r="N30" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O30" s="7"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+    </row>
+    <row r="31" spans="2:31" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="7"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -955,22 +1384,244 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:18" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
+    <row r="32" spans="2:31" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="N32" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="O32" s="11"/>
+      <c r="P32" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q32" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R32" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="S32" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="T32" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="U32" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="V32" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="W32" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="X32" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y32" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z32" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA32" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="2:27" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="N33" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="O33" s="7"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="5"/>
+    </row>
+    <row r="34" spans="2:27" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N34" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="O34" s="7"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="5"/>
+      <c r="X34" s="5"/>
+      <c r="Y34" s="5"/>
+      <c r="Z34" s="5"/>
+      <c r="AA34" s="5"/>
+    </row>
+    <row r="35" spans="2:27" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N35" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O35" s="7"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="5"/>
+    </row>
+    <row r="36" spans="2:27" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="O36" s="7"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
+      <c r="Y36" s="5"/>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5"/>
+    </row>
+    <row r="37" spans="2:27" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="N37" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O37" s="7"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="5"/>
+      <c r="V37" s="5"/>
+      <c r="W37" s="5"/>
+      <c r="X37" s="5"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="5"/>
+    </row>
+    <row r="38" spans="2:27" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="40">
+    <mergeCell ref="AE24:AE25"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="V24:V25"/>
+    <mergeCell ref="W24:W25"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="Y24:Y25"/>
+    <mergeCell ref="Z24:Z25"/>
+    <mergeCell ref="AA24:AA25"/>
+    <mergeCell ref="AB24:AB25"/>
+    <mergeCell ref="AC24:AC25"/>
+    <mergeCell ref="AD24:AD25"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N24:O25"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B26:C26"/>
@@ -978,7 +1629,6 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>